<commit_message>
new data and scripts
</commit_message>
<xml_diff>
--- a/02_outputs/pesquisas-infos.xlsx
+++ b/02_outputs/pesquisas-infos.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>9-2014</t>
+          <t>09-2014</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>9-2014</t>
+          <t>09-2014</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>9-2014</t>
+          <t>09-2014</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -7144,6 +7144,378 @@
       <c r="L110" t="inlineStr">
         <is>
           <t>2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Não sabe</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Concorda totalmente</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>602</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>Concorda em parte</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>Discorda em parte</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>Nem concorda, nem discorda</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>04843</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Data Folha</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>PERFIL IDEOLÓGICO</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>06-2023</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Eleitores de 16 anos ou mais</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>p901a</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>P.901 Agora vou ler algumas frases e gostaria que você me dissesse se concorda ou discorda de cada uma delas. - Possuir arma legalizada deveria ser um direito do cidadão para se defender</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>Discorda totalmente</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>803</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>2010</t>
         </is>
       </c>
     </row>

</xml_diff>